<commit_message>
working code for suppression check + insertion
</commit_message>
<xml_diff>
--- a/uploads/insert-newrecords.xlsx
+++ b/uploads/insert-newrecords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prajwal.pawar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5696C159-EE04-475F-BF11-8F927CDC8E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52A18E1-B30E-4CF7-8398-6B08DC57434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39C0FAAC-3DCF-4200-BE2B-520D72FC70FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="104">
   <si>
     <t>Date_</t>
   </si>
@@ -342,6 +342,12 @@
   </si>
   <si>
     <t>ChadKrasPubl</t>
+  </si>
+  <si>
+    <t>ChaKraPuba</t>
+  </si>
+  <si>
+    <t>ChadKrasPubla</t>
   </si>
 </sst>
 </file>
@@ -771,13 +777,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8446F0D6-4625-419A-9772-100C1625C0AC}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -837,7 +846,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>45302</v>
+        <v>45423</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>18</v>
@@ -1117,7 +1126,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>45302</v>
+        <v>45576</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>18</v>
@@ -1397,7 +1406,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>45302</v>
+        <v>44572</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>18</v>
@@ -1504,6 +1513,62 @@
         <v>40</v>
       </c>
       <c r="R13" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>45668</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="6">
+        <v>9391</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="7">
+        <v>2142440955</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R14" s="8" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>